<commit_message>
improve vectordb, add location search, generate embeddings batch script, reset vectorbdb
</commit_message>
<xml_diff>
--- a/research-contacts-progress.xlsx
+++ b/research-contacts-progress.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3460"/>
+  <dimension ref="A1:I3461"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -89087,9 +89087,35 @@
         <v>In Progress</v>
       </c>
     </row>
+    <row r="3461">
+      <c r="A3461" t="str">
+        <v>2025-07-30T06:29:00.735Z</v>
+      </c>
+      <c r="B3461">
+        <v>1</v>
+      </c>
+      <c r="C3461" t="str">
+        <v>0/0</v>
+      </c>
+      <c r="D3461">
+        <v>0</v>
+      </c>
+      <c r="E3461">
+        <v>0</v>
+      </c>
+      <c r="F3461">
+        <v>0</v>
+      </c>
+      <c r="G3461" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3461" t="str">
+        <v>In Progress</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I3460"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I3461"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>